<commit_message>
comma separator on bundle item list on flash template; adjust cell width on flash template
</commit_message>
<xml_diff>
--- a/templates/flash.xlsx
+++ b/templates/flash.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sample-projects\edge-system\edge-node\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ennovation\edge-system\edge-node\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -710,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2:L2"/>
     </sheetView>
@@ -719,14 +719,18 @@
   <cols>
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="23.21875" customWidth="1"/>
     <col min="9" max="9" width="8.5546875" customWidth="1"/>
     <col min="10" max="12" width="7.109375" customWidth="1"/>
-    <col min="13" max="26" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="21.77734375" customWidth="1"/>
+    <col min="14" max="14" width="39" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="16" max="26" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.75" customHeight="1">

</xml_diff>